<commit_message>
City index 25-10 7/12
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_18952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_18952.xlsx
@@ -2649,6 +2649,9 @@
       <c r="M3">
         <v>-0.44</v>
       </c>
+      <c r="N3">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2752,6 +2755,9 @@
       <c r="M5">
         <v>1.69</v>
       </c>
+      <c r="N5">
+        <v>0.53</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2937,6 +2943,9 @@
       <c r="M9">
         <v>3.03</v>
       </c>
+      <c r="N9">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3034,6 +3043,9 @@
       <c r="M11">
         <v>5.98</v>
       </c>
+      <c r="N11">
+        <v>5.51</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3137,6 +3149,9 @@
       <c r="M13">
         <v>-0.99</v>
       </c>
+      <c r="N13">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3313,6 +3328,9 @@
       <c r="M17">
         <v>0.26</v>
       </c>
+      <c r="N17">
+        <v>-0.8</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3416,6 +3434,9 @@
       <c r="M19">
         <v>4.97</v>
       </c>
+      <c r="N19">
+        <v>1.02</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3516,6 +3537,9 @@
       <c r="M21">
         <v>8.470000000000001</v>
       </c>
+      <c r="N21">
+        <v>12.73</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3610,6 +3634,9 @@
       <c r="L23">
         <v>-0.06</v>
       </c>
+      <c r="N23">
+        <v>-2.52</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3707,6 +3734,9 @@
       <c r="M25">
         <v>-2.07</v>
       </c>
+      <c r="N25">
+        <v>-3.08</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3810,6 +3840,9 @@
       <c r="M27">
         <v>6.64</v>
       </c>
+      <c r="N27">
+        <v>8.869999999999999</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3913,6 +3946,9 @@
       <c r="M29">
         <v>3.21</v>
       </c>
+      <c r="N29">
+        <v>-0.49</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4016,6 +4052,9 @@
       <c r="M31">
         <v>0.55</v>
       </c>
+      <c r="N31">
+        <v>1.64</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4119,6 +4158,9 @@
       <c r="M33">
         <v>2.47</v>
       </c>
+      <c r="N33">
+        <v>2.66</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4216,6 +4258,9 @@
       <c r="L35">
         <v>2.23</v>
       </c>
+      <c r="N35">
+        <v>-0.03</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4359,6 +4404,9 @@
       <c r="M39">
         <v>4.6</v>
       </c>
+      <c r="N39">
+        <v>4.99</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4462,6 +4510,9 @@
       <c r="M41">
         <v>0.99</v>
       </c>
+      <c r="N41">
+        <v>4.09</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4565,6 +4616,9 @@
       <c r="M43">
         <v>-0.45</v>
       </c>
+      <c r="N43">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4659,6 +4713,9 @@
       <c r="M45">
         <v>6.95</v>
       </c>
+      <c r="N45">
+        <v>5.54</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4762,6 +4819,9 @@
       <c r="M47">
         <v>-0.87</v>
       </c>
+      <c r="N47">
+        <v>1.69</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4941,6 +5001,9 @@
       <c r="M51">
         <v>1.49</v>
       </c>
+      <c r="N51">
+        <v>2.6</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5041,6 +5104,9 @@
       <c r="M53">
         <v>19.38</v>
       </c>
+      <c r="N53">
+        <v>17.48</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5137,6 +5203,9 @@
       </c>
       <c r="L55">
         <v>1.93</v>
+      </c>
+      <c r="N55">
+        <v>2.14</v>
       </c>
     </row>
   </sheetData>
@@ -5244,7 +5313,7 @@
         <v>26</v>
       </c>
       <c r="G2">
-        <v>0.9629716560401228</v>
+        <v>0.9676465159429686</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -5286,19 +5355,19 @@
         <v>2025</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>1.0196</v>
+        <v>1.0204</v>
       </c>
       <c r="F3">
         <v>25</v>
       </c>
       <c r="G3">
-        <v>0.9699107532353879</v>
+        <v>0.9687275452614585</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -5317,12 +5386,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>sep</t>
+          <t>okt</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>jan-sep</t>
+          <t>jan-okt</t>
         </is>
       </c>
       <c r="M3">
@@ -5339,7 +5408,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5822,10 +5891,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.9991540139922993</v>
+        <v>0.9991532249526388</v>
       </c>
       <c r="B11">
-        <v>-0.08459860077006942</v>
+        <v>-0.08467750473611924</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -5834,10 +5903,10 @@
         <v>15.71971180997949</v>
       </c>
       <c r="E11">
-        <v>5.216640705860183</v>
+        <v>5.216467590334918</v>
       </c>
       <c r="F11">
-        <v>1.315735631396686</v>
+        <v>1.315691968381006</v>
       </c>
       <c r="G11">
         <v>-2.8</v>
@@ -5860,6 +5929,51 @@
         <v>2025</v>
       </c>
       <c r="M11" t="inlineStr">
+        <is>
+          <t>12_months</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>1.001402751121869</v>
+      </c>
+      <c r="B12">
+        <v>0.1402751121869494</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>15.71971180997949</v>
+      </c>
+      <c r="E12">
+        <v>5.326593606543288</v>
+      </c>
+      <c r="F12">
+        <v>1.343467836346448</v>
+      </c>
+      <c r="G12">
+        <v>-2.7</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2023 - (nov 2024 - okt 2025)</t>
+        </is>
+      </c>
+      <c r="J12" s="2">
+        <v>45931</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>2025</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>12_months</t>
         </is>

</xml_diff>

<commit_message>
City index 25 7/12. Added table for last 36 trp.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_18952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_18952.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Programmering\R\byindeks\data_indexpoints_tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17CE747-4C2C-4C43-8497-2F7B835562B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E076C53-AE29-4094-B759-C3223034BE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="38610" windowHeight="20985" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="205">
   <si>
     <t>trp_id</t>
   </si>
@@ -182,7 +182,7 @@
     <t>08132V1984223</t>
   </si>
   <si>
-    <t>Værstebrua</t>
+    <t>Værstebroa</t>
   </si>
   <si>
     <t>FV108 S1D1 m1071</t>
@@ -275,7 +275,7 @@
     <t>Hauge bru</t>
   </si>
   <si>
-    <t>FV112 S1D1 m7437</t>
+    <t>FV112 S1D1 m7436</t>
   </si>
   <si>
     <t>fv. 112</t>
@@ -566,9 +566,6 @@
     <t>2024-2025</t>
   </si>
   <si>
-    <t>jan-nov</t>
-  </si>
-  <si>
     <t>chained</t>
   </si>
   <si>
@@ -633,6 +630,15 @@
   </si>
   <si>
     <t>2023 - (des 2024 - nov 2025)</t>
+  </si>
+  <si>
+    <t>2023 - (jan 2025 - des 2025)</t>
+  </si>
+  <si>
+    <t>2023 - (jan 2024 - des 2025)</t>
+  </si>
+  <si>
+    <t>24_months</t>
   </si>
 </sst>
 </file>
@@ -991,13 +997,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1082,10 +1086,10 @@
         <v>24</v>
       </c>
       <c r="K2">
-        <v>11330</v>
+        <v>11490</v>
       </c>
       <c r="L2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M2">
         <v>11260</v>
@@ -1097,13 +1101,13 @@
         <v>1970</v>
       </c>
       <c r="P2">
-        <v>12390</v>
+        <v>12620</v>
       </c>
       <c r="Q2">
-        <v>1940</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1135,10 +1139,10 @@
         <v>24</v>
       </c>
       <c r="K3">
-        <v>8400</v>
+        <v>8620</v>
       </c>
       <c r="L3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M3">
         <v>8750</v>
@@ -1150,13 +1154,13 @@
         <v>1730</v>
       </c>
       <c r="P3">
-        <v>9380</v>
+        <v>9590</v>
       </c>
       <c r="Q3">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1188,10 +1192,10 @@
         <v>24</v>
       </c>
       <c r="K4">
-        <v>10520</v>
+        <v>10530</v>
       </c>
       <c r="L4">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M4">
         <v>11300</v>
@@ -1203,13 +1207,13 @@
         <v>1900</v>
       </c>
       <c r="P4">
-        <v>11700</v>
+        <v>11680</v>
       </c>
       <c r="Q4">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1232,7 +1236,7 @@
         <v>59.272764000000002</v>
       </c>
       <c r="H5">
-        <v>11.143732999999999</v>
+        <v>11.14373</v>
       </c>
       <c r="I5" t="s">
         <v>37</v>
@@ -1262,7 +1266,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1294,10 +1298,10 @@
         <v>24</v>
       </c>
       <c r="K6">
-        <v>23030</v>
+        <v>23650</v>
       </c>
       <c r="L6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M6">
         <v>22930</v>
@@ -1309,13 +1313,13 @@
         <v>2110</v>
       </c>
       <c r="P6">
-        <v>25050</v>
+        <v>25700</v>
       </c>
       <c r="Q6">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1347,10 +1351,10 @@
         <v>24</v>
       </c>
       <c r="K7">
-        <v>19080</v>
+        <v>17910</v>
       </c>
       <c r="L7">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M7">
         <v>17140</v>
@@ -1362,13 +1366,13 @@
         <v>1590</v>
       </c>
       <c r="P7">
-        <v>20770</v>
+        <v>19560</v>
       </c>
       <c r="Q7">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1400,10 +1404,10 @@
         <v>24</v>
       </c>
       <c r="K8">
-        <v>24630</v>
+        <v>24970</v>
       </c>
       <c r="L8">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M8">
         <v>24770</v>
@@ -1415,13 +1419,13 @@
         <v>2540</v>
       </c>
       <c r="P8">
-        <v>27070</v>
+        <v>27420</v>
       </c>
       <c r="Q8">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1453,10 +1457,10 @@
         <v>24</v>
       </c>
       <c r="K9">
-        <v>10970</v>
+        <v>12610</v>
       </c>
       <c r="L9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M9">
         <v>11260</v>
@@ -1468,13 +1472,13 @@
         <v>910</v>
       </c>
       <c r="P9">
-        <v>12280</v>
+        <v>14050</v>
       </c>
       <c r="Q9">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1494,10 +1498,10 @@
         <v>22</v>
       </c>
       <c r="G10">
-        <v>59.207855000000002</v>
+        <v>59.207853999999998</v>
       </c>
       <c r="H10">
-        <v>10.93777</v>
+        <v>10.937768999999999</v>
       </c>
       <c r="I10" t="s">
         <v>59</v>
@@ -1506,10 +1510,10 @@
         <v>24</v>
       </c>
       <c r="K10">
-        <v>12190</v>
+        <v>13170</v>
       </c>
       <c r="L10">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M10">
         <v>11710</v>
@@ -1521,13 +1525,13 @@
         <v>630</v>
       </c>
       <c r="P10">
-        <v>13440</v>
+        <v>14480</v>
       </c>
       <c r="Q10">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1559,10 +1563,10 @@
         <v>24</v>
       </c>
       <c r="K11">
-        <v>22980</v>
+        <v>23150</v>
       </c>
       <c r="L11">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M11">
         <v>23550</v>
@@ -1574,13 +1578,13 @@
         <v>2140</v>
       </c>
       <c r="P11">
-        <v>25980</v>
+        <v>26180</v>
       </c>
       <c r="Q11">
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -1612,10 +1616,10 @@
         <v>24</v>
       </c>
       <c r="K12">
-        <v>23160</v>
+        <v>23000</v>
       </c>
       <c r="L12">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M12">
         <v>23420</v>
@@ -1627,13 +1631,13 @@
         <v>1980</v>
       </c>
       <c r="P12">
-        <v>26110</v>
+        <v>25880</v>
       </c>
       <c r="Q12">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1665,10 +1669,10 @@
         <v>24</v>
       </c>
       <c r="K13">
-        <v>14920</v>
+        <v>14990</v>
       </c>
       <c r="L13">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M13">
         <v>15250</v>
@@ -1680,13 +1684,13 @@
         <v>1620</v>
       </c>
       <c r="P13">
-        <v>16570</v>
+        <v>16640</v>
       </c>
       <c r="Q13">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1718,10 +1722,10 @@
         <v>24</v>
       </c>
       <c r="K14">
-        <v>6230</v>
+        <v>6070</v>
       </c>
       <c r="L14">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M14">
         <v>6050</v>
@@ -1733,13 +1737,13 @@
         <v>660</v>
       </c>
       <c r="P14">
-        <v>7190</v>
+        <v>6940</v>
       </c>
       <c r="Q14">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1771,10 +1775,10 @@
         <v>24</v>
       </c>
       <c r="K15">
-        <v>8080</v>
+        <v>7690</v>
       </c>
       <c r="L15">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M15">
         <v>7240</v>
@@ -1786,13 +1790,13 @@
         <v>500</v>
       </c>
       <c r="P15">
-        <v>8850</v>
+        <v>8420</v>
       </c>
       <c r="Q15">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1815,7 +1819,7 @@
         <v>59.322237000000001</v>
       </c>
       <c r="H16">
-        <v>10.957967</v>
+        <v>10.957966000000001</v>
       </c>
       <c r="I16" t="s">
         <v>85</v>
@@ -1824,10 +1828,10 @@
         <v>24</v>
       </c>
       <c r="K16">
-        <v>3910</v>
+        <v>4000</v>
       </c>
       <c r="L16">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M16">
         <v>3900</v>
@@ -1839,13 +1843,13 @@
         <v>860</v>
       </c>
       <c r="P16">
-        <v>4480</v>
+        <v>4580</v>
       </c>
       <c r="Q16">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -1877,10 +1881,10 @@
         <v>24</v>
       </c>
       <c r="K17">
-        <v>5190</v>
+        <v>4810</v>
       </c>
       <c r="L17">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M17">
         <v>4350</v>
@@ -1892,13 +1896,13 @@
         <v>240</v>
       </c>
       <c r="P17">
-        <v>5960</v>
+        <v>5510</v>
       </c>
       <c r="Q17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1930,10 +1934,10 @@
         <v>24</v>
       </c>
       <c r="K18">
-        <v>2870</v>
+        <v>2970</v>
       </c>
       <c r="L18">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M18">
         <v>2990</v>
@@ -1945,13 +1949,13 @@
         <v>360</v>
       </c>
       <c r="P18">
-        <v>3190</v>
+        <v>3270</v>
       </c>
       <c r="Q18">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -1983,10 +1987,10 @@
         <v>24</v>
       </c>
       <c r="K19">
-        <v>5660</v>
+        <v>5780</v>
       </c>
       <c r="L19">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M19">
         <v>5600</v>
@@ -1998,13 +2002,13 @@
         <v>530</v>
       </c>
       <c r="P19">
-        <v>6120</v>
+        <v>6240</v>
       </c>
       <c r="Q19">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -2036,10 +2040,10 @@
         <v>24</v>
       </c>
       <c r="K20">
-        <v>8120</v>
+        <v>8430</v>
       </c>
       <c r="L20">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M20">
         <v>8150</v>
@@ -2051,13 +2055,13 @@
         <v>600</v>
       </c>
       <c r="P20">
-        <v>8710</v>
+        <v>9060</v>
       </c>
       <c r="Q20">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -2077,10 +2081,10 @@
         <v>32</v>
       </c>
       <c r="G21">
-        <v>59.213293</v>
+        <v>59.213293999999998</v>
       </c>
       <c r="H21">
-        <v>11.189306999999999</v>
+        <v>11.189306</v>
       </c>
       <c r="I21" t="s">
         <v>109</v>
@@ -2089,10 +2093,10 @@
         <v>24</v>
       </c>
       <c r="K21">
-        <v>5470</v>
+        <v>5620</v>
       </c>
       <c r="L21">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M21">
         <v>5130</v>
@@ -2104,13 +2108,13 @@
         <v>380</v>
       </c>
       <c r="P21">
-        <v>5900</v>
+        <v>6070</v>
       </c>
       <c r="Q21">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>110</v>
       </c>
@@ -2142,10 +2146,10 @@
         <v>24</v>
       </c>
       <c r="K22">
-        <v>17710</v>
+        <v>17730</v>
       </c>
       <c r="L22">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M22">
         <v>19410</v>
@@ -2160,10 +2164,10 @@
         <v>19360</v>
       </c>
       <c r="Q22">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -2195,10 +2199,10 @@
         <v>24</v>
       </c>
       <c r="K23">
-        <v>12720</v>
+        <v>12930</v>
       </c>
       <c r="L23">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M23">
         <v>13840</v>
@@ -2210,13 +2214,13 @@
         <v>1320</v>
       </c>
       <c r="P23">
-        <v>14270</v>
+        <v>14520</v>
       </c>
       <c r="Q23">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -2248,10 +2252,10 @@
         <v>24</v>
       </c>
       <c r="K24">
-        <v>10720</v>
+        <v>11380</v>
       </c>
       <c r="L24">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M24">
         <v>10860</v>
@@ -2263,13 +2267,13 @@
         <v>1240</v>
       </c>
       <c r="P24">
-        <v>11620</v>
+        <v>12320</v>
       </c>
       <c r="Q24">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -2301,10 +2305,10 @@
         <v>24</v>
       </c>
       <c r="K25">
-        <v>9640</v>
+        <v>9860</v>
       </c>
       <c r="L25">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M25">
         <v>9740</v>
@@ -2316,13 +2320,13 @@
         <v>890</v>
       </c>
       <c r="P25">
-        <v>10570</v>
+        <v>10760</v>
       </c>
       <c r="Q25">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -2354,10 +2358,10 @@
         <v>24</v>
       </c>
       <c r="K26">
-        <v>6580</v>
+        <v>7140</v>
       </c>
       <c r="L26">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M26">
         <v>7000</v>
@@ -2369,13 +2373,13 @@
         <v>550</v>
       </c>
       <c r="P26">
-        <v>6970</v>
+        <v>7540</v>
       </c>
       <c r="Q26">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>59.215721000000002</v>
       </c>
       <c r="H27">
-        <v>11.180446</v>
+        <v>11.180446999999999</v>
       </c>
       <c r="I27" t="s">
         <v>134</v>
@@ -2407,10 +2411,10 @@
         <v>24</v>
       </c>
       <c r="K27">
-        <v>5350</v>
+        <v>5440</v>
       </c>
       <c r="L27">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M27">
         <v>5180</v>
@@ -2422,13 +2426,13 @@
         <v>510</v>
       </c>
       <c r="P27">
-        <v>5760</v>
+        <v>5860</v>
       </c>
       <c r="Q27">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -2460,10 +2464,10 @@
         <v>24</v>
       </c>
       <c r="K28">
-        <v>6180</v>
+        <v>6150</v>
       </c>
       <c r="L28">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M28">
         <v>6360</v>
@@ -2475,13 +2479,13 @@
         <v>380</v>
       </c>
       <c r="P28">
-        <v>6830</v>
+        <v>6770</v>
       </c>
       <c r="Q28">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -2501,10 +2505,10 @@
         <v>22</v>
       </c>
       <c r="G29">
-        <v>59.282975</v>
+        <v>59.282975999999998</v>
       </c>
       <c r="H29">
-        <v>10.939785000000001</v>
+        <v>10.939786</v>
       </c>
       <c r="I29" t="s">
         <v>143</v>
@@ -2513,10 +2517,10 @@
         <v>24</v>
       </c>
       <c r="K29">
-        <v>2260</v>
+        <v>2240</v>
       </c>
       <c r="L29">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M29">
         <v>2480</v>
@@ -2528,13 +2532,13 @@
         <v>250</v>
       </c>
       <c r="P29">
-        <v>2620</v>
+        <v>2580</v>
       </c>
       <c r="Q29">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -2557,7 +2561,7 @@
         <v>59.277749</v>
       </c>
       <c r="H30">
-        <v>11.136839</v>
+        <v>11.136839999999999</v>
       </c>
       <c r="I30" t="s">
         <v>148</v>
@@ -2566,10 +2570,10 @@
         <v>24</v>
       </c>
       <c r="K30">
-        <v>6670</v>
+        <v>6940</v>
       </c>
       <c r="L30">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M30">
         <v>6960</v>
@@ -2581,10 +2585,10 @@
         <v>780</v>
       </c>
       <c r="P30">
-        <v>7250</v>
+        <v>7530</v>
       </c>
       <c r="Q30">
-        <v>700</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -2594,13 +2598,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2700,7 +2704,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -2746,8 +2750,11 @@
       <c r="O3">
         <v>-1.79</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P3">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2797,7 +2804,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2843,8 +2850,11 @@
       <c r="O5">
         <v>-0.41</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2885,7 +2895,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -2916,8 +2926,11 @@
       <c r="O7">
         <v>-1.24</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P7">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -2967,7 +2980,7 @@
         <v>-3.67</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -3013,8 +3026,11 @@
       <c r="O9">
         <v>4.18</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P9">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -3058,7 +3074,7 @@
         <v>-2.4500000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -3104,8 +3120,11 @@
       <c r="O11">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P11">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3155,7 +3174,7 @@
         <v>-6.61</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -3201,8 +3220,11 @@
       <c r="O13">
         <v>-1.81</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P13">
+        <v>4.6900000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3252,7 +3274,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3266,7 +3288,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -3316,7 +3338,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -3359,8 +3381,11 @@
       <c r="O17">
         <v>-2.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P17">
+        <v>-0.37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3410,7 +3435,7 @@
         <v>-4.1500000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3456,8 +3481,11 @@
       <c r="O19">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P19">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3507,7 +3535,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3550,8 +3578,11 @@
       <c r="O21">
         <v>5.24</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P21">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -3598,7 +3629,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -3638,8 +3669,11 @@
       <c r="O23">
         <v>-3.12</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P23">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -3683,7 +3717,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -3729,8 +3763,11 @@
       <c r="O25">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P25">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>118</v>
       </c>
@@ -3780,7 +3817,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -3826,8 +3863,11 @@
       <c r="O27">
         <v>3.31</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P27">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3877,7 +3917,7 @@
         <v>-2.2200000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3921,7 +3961,7 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -3971,7 +4011,7 @@
         <v>-6.35</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4017,8 +4057,11 @@
       <c r="O31">
         <v>-0.67</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P31">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -4068,7 +4111,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -4114,8 +4157,11 @@
       <c r="O33">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P33">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -4162,7 +4208,7 @@
         <v>11.93</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -4205,8 +4251,11 @@
       <c r="O35">
         <v>-2.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P35">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -4250,7 +4299,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -4290,13 +4339,16 @@
       <c r="O37">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P37">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
         <v>121</v>
@@ -4304,13 +4356,49 @@
       <c r="D38">
         <v>2024</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <v>5.64</v>
+      </c>
+      <c r="F38">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G38">
+        <v>6.62</v>
+      </c>
+      <c r="H38">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="I38">
+        <v>7.43</v>
+      </c>
+      <c r="J38">
+        <v>-5.77</v>
+      </c>
+      <c r="K38">
+        <v>5.82</v>
+      </c>
+      <c r="L38">
+        <v>5.71</v>
+      </c>
+      <c r="M38">
+        <v>-0.9</v>
+      </c>
+      <c r="N38">
+        <v>0.22</v>
+      </c>
+      <c r="O38">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="P38">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
         <v>121</v>
@@ -4318,742 +4406,687 @@
       <c r="D39">
         <v>2025</v>
       </c>
+      <c r="E39">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="F39">
+        <v>-1.86</v>
+      </c>
+      <c r="G39">
+        <v>2.12</v>
+      </c>
+      <c r="H39">
+        <v>1.29</v>
+      </c>
+      <c r="I39">
+        <v>-6.63</v>
+      </c>
+      <c r="J39">
+        <v>0.25</v>
+      </c>
       <c r="K39">
-        <v>9.7200000000000006</v>
+        <v>13.09</v>
       </c>
       <c r="L39">
-        <v>5.72</v>
+        <v>0.36</v>
       </c>
       <c r="M39">
-        <v>4.5999999999999996</v>
+        <v>0.99</v>
       </c>
       <c r="N39">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.09</v>
+      </c>
+      <c r="O39">
+        <v>0.31</v>
+      </c>
+      <c r="P39">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="D40">
         <v>2024</v>
       </c>
       <c r="E40">
-        <v>5.64</v>
+        <v>6.35</v>
       </c>
       <c r="F40">
-        <v>8.1199999999999992</v>
+        <v>6.78</v>
       </c>
       <c r="G40">
-        <v>6.62</v>
+        <v>-2.94</v>
       </c>
       <c r="H40">
-        <v>9.3699999999999992</v>
+        <v>9.44</v>
       </c>
       <c r="I40">
-        <v>7.43</v>
+        <v>1.36</v>
       </c>
       <c r="J40">
-        <v>-5.77</v>
+        <v>-5.96</v>
       </c>
       <c r="K40">
-        <v>5.82</v>
+        <v>-4.2699999999999996</v>
       </c>
       <c r="L40">
-        <v>5.71</v>
+        <v>-6</v>
       </c>
       <c r="M40">
-        <v>-0.9</v>
+        <v>-4.74</v>
       </c>
       <c r="N40">
-        <v>0.22</v>
+        <v>-1.35</v>
       </c>
       <c r="O40">
-        <v>-0.56000000000000005</v>
+        <v>-4.8499999999999996</v>
       </c>
       <c r="P40">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-4.41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="D41">
         <v>2025</v>
       </c>
       <c r="E41">
-        <v>-0.28000000000000003</v>
+        <v>-2.85</v>
       </c>
       <c r="F41">
-        <v>-1.86</v>
+        <v>-5.42</v>
       </c>
       <c r="G41">
-        <v>2.12</v>
+        <v>2.81</v>
       </c>
       <c r="H41">
-        <v>1.29</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="I41">
-        <v>-6.63</v>
+        <v>1.05</v>
       </c>
       <c r="J41">
-        <v>0.25</v>
+        <v>-0.44</v>
       </c>
       <c r="K41">
-        <v>13.09</v>
+        <v>0.51</v>
       </c>
       <c r="L41">
-        <v>0.36</v>
+        <v>-1.01</v>
       </c>
       <c r="M41">
-        <v>0.99</v>
+        <v>-0.45</v>
       </c>
       <c r="N41">
-        <v>4.09</v>
+        <v>0.1</v>
       </c>
       <c r="O41">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-0.35</v>
+      </c>
+      <c r="P41">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D42">
         <v>2024</v>
       </c>
       <c r="E42">
-        <v>6.35</v>
+        <v>-13.07</v>
       </c>
       <c r="F42">
-        <v>6.78</v>
+        <v>-9.4600000000000009</v>
       </c>
       <c r="G42">
-        <v>-2.94</v>
+        <v>-10.3</v>
       </c>
       <c r="H42">
-        <v>9.44</v>
-      </c>
-      <c r="I42">
-        <v>1.36</v>
-      </c>
-      <c r="J42">
-        <v>-5.96</v>
-      </c>
-      <c r="K42">
-        <v>-4.2699999999999996</v>
+        <v>9.98</v>
       </c>
       <c r="L42">
-        <v>-6</v>
+        <v>-5.88</v>
       </c>
       <c r="M42">
-        <v>-4.74</v>
+        <v>-5.34</v>
       </c>
       <c r="N42">
-        <v>-1.35</v>
+        <v>-4.37</v>
       </c>
       <c r="O42">
-        <v>-4.8499999999999996</v>
+        <v>-2.09</v>
       </c>
       <c r="P42">
-        <v>-4.41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-6.68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43">
+        <v>2025</v>
+      </c>
+      <c r="E43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F43">
+        <v>-1.44</v>
+      </c>
+      <c r="G43">
+        <v>1.22</v>
+      </c>
+      <c r="H43">
+        <v>-3.89</v>
+      </c>
+      <c r="I43">
+        <v>-0.34</v>
+      </c>
+      <c r="J43">
+        <v>3.24</v>
+      </c>
+      <c r="K43">
+        <v>5.01</v>
+      </c>
+      <c r="L43">
+        <v>8.14</v>
+      </c>
+      <c r="M43">
+        <v>6.95</v>
+      </c>
+      <c r="N43">
+        <v>5.54</v>
+      </c>
+      <c r="O43">
+        <v>0.67</v>
+      </c>
+      <c r="P43">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
         <v>63</v>
-      </c>
-      <c r="D43">
-        <v>2025</v>
-      </c>
-      <c r="E43">
-        <v>-2.85</v>
-      </c>
-      <c r="F43">
-        <v>-5.42</v>
-      </c>
-      <c r="G43">
-        <v>2.81</v>
-      </c>
-      <c r="H43">
-        <v>-4.4000000000000004</v>
-      </c>
-      <c r="I43">
-        <v>1.05</v>
-      </c>
-      <c r="J43">
-        <v>-0.44</v>
-      </c>
-      <c r="K43">
-        <v>0.51</v>
-      </c>
-      <c r="L43">
-        <v>-1.01</v>
-      </c>
-      <c r="M43">
-        <v>-0.45</v>
-      </c>
-      <c r="N43">
-        <v>0.1</v>
-      </c>
-      <c r="O43">
-        <v>-0.35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
       </c>
       <c r="D44">
         <v>2024</v>
       </c>
       <c r="E44">
-        <v>-13.07</v>
+        <v>-1.17</v>
       </c>
       <c r="F44">
-        <v>-9.4600000000000009</v>
+        <v>5.26</v>
       </c>
       <c r="G44">
-        <v>-10.3</v>
+        <v>6.7</v>
       </c>
       <c r="H44">
-        <v>9.98</v>
+        <v>18.690000000000001</v>
+      </c>
+      <c r="I44">
+        <v>52.17</v>
+      </c>
+      <c r="J44">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="K44">
+        <v>9.58</v>
       </c>
       <c r="L44">
-        <v>-5.88</v>
+        <v>9.52</v>
       </c>
       <c r="M44">
-        <v>-5.34</v>
+        <v>3.92</v>
       </c>
       <c r="N44">
-        <v>-4.37</v>
+        <v>7.23</v>
       </c>
       <c r="O44">
-        <v>-2.09</v>
+        <v>1.63</v>
       </c>
       <c r="P44">
-        <v>-6.68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D45">
         <v>2025</v>
       </c>
       <c r="E45">
-        <v>2.2000000000000002</v>
+        <v>3.52</v>
       </c>
       <c r="F45">
-        <v>-1.44</v>
+        <v>-3.81</v>
       </c>
       <c r="G45">
-        <v>1.22</v>
+        <v>-10.18</v>
       </c>
       <c r="H45">
-        <v>-3.89</v>
+        <v>-15.61</v>
       </c>
       <c r="I45">
-        <v>-0.34</v>
+        <v>-10.44</v>
       </c>
       <c r="J45">
-        <v>3.24</v>
+        <v>-9.64</v>
       </c>
       <c r="K45">
-        <v>5.01</v>
+        <v>-6.59</v>
       </c>
       <c r="L45">
-        <v>8.14</v>
+        <v>-8.06</v>
       </c>
       <c r="M45">
-        <v>6.95</v>
+        <v>-0.87</v>
       </c>
       <c r="N45">
-        <v>5.54</v>
+        <v>1.69</v>
       </c>
       <c r="O45">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.24</v>
+      </c>
+      <c r="P45">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="D46">
         <v>2024</v>
       </c>
       <c r="E46">
-        <v>-1.17</v>
+        <v>-5.76</v>
       </c>
       <c r="F46">
-        <v>5.26</v>
+        <v>-3.06</v>
       </c>
       <c r="G46">
-        <v>6.7</v>
+        <v>-10.41</v>
       </c>
       <c r="H46">
-        <v>18.690000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="I46">
-        <v>52.17</v>
+        <v>-13.03</v>
       </c>
       <c r="J46">
-        <v>39.909999999999997</v>
+        <v>-16.21</v>
       </c>
       <c r="K46">
-        <v>9.58</v>
+        <v>-7.98</v>
       </c>
       <c r="L46">
-        <v>9.52</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="M46">
-        <v>3.92</v>
+        <v>-7.98</v>
       </c>
       <c r="N46">
-        <v>7.23</v>
+        <v>-6.68</v>
       </c>
       <c r="O46">
-        <v>1.63</v>
+        <v>-8.2200000000000006</v>
       </c>
       <c r="P46">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-5.26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="D47">
         <v>2025</v>
       </c>
-      <c r="E47">
-        <v>3.52</v>
-      </c>
-      <c r="F47">
-        <v>-3.81</v>
-      </c>
-      <c r="G47">
-        <v>-10.18</v>
-      </c>
-      <c r="H47">
-        <v>-15.61</v>
-      </c>
-      <c r="I47">
-        <v>-10.44</v>
-      </c>
-      <c r="J47">
-        <v>-9.64</v>
-      </c>
-      <c r="K47">
-        <v>-6.59</v>
-      </c>
-      <c r="L47">
-        <v>-8.06</v>
-      </c>
-      <c r="M47">
-        <v>-0.87</v>
-      </c>
-      <c r="N47">
-        <v>1.69</v>
-      </c>
-      <c r="O47">
-        <v>1.24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D48">
         <v>2024</v>
       </c>
       <c r="E48">
-        <v>-5.76</v>
+        <v>5.92</v>
       </c>
       <c r="F48">
-        <v>-3.06</v>
+        <v>7.23</v>
       </c>
       <c r="G48">
-        <v>-10.41</v>
+        <v>-3.77</v>
       </c>
       <c r="H48">
-        <v>-0.28999999999999998</v>
+        <v>8.68</v>
       </c>
       <c r="I48">
-        <v>-13.03</v>
+        <v>-2.65</v>
       </c>
       <c r="J48">
-        <v>-16.21</v>
+        <v>-11.03</v>
       </c>
       <c r="K48">
-        <v>-7.98</v>
+        <v>-9.7899999999999991</v>
       </c>
       <c r="L48">
-        <v>-9.6999999999999993</v>
+        <v>-5.31</v>
       </c>
       <c r="M48">
-        <v>-7.98</v>
+        <v>-4.5</v>
       </c>
       <c r="N48">
-        <v>-6.68</v>
+        <v>-3.04</v>
       </c>
       <c r="O48">
-        <v>-8.2200000000000006</v>
+        <v>-8.1</v>
       </c>
       <c r="P48">
-        <v>-5.26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-5.0599999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D49">
         <v>2025</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E49">
+        <v>-8</v>
+      </c>
+      <c r="F49">
+        <v>-7.24</v>
+      </c>
+      <c r="G49">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="H49">
+        <v>-4.91</v>
+      </c>
+      <c r="I49">
+        <v>0.13</v>
+      </c>
+      <c r="J49">
+        <v>3.01</v>
+      </c>
+      <c r="K49">
+        <v>0.95</v>
+      </c>
+      <c r="L49">
+        <v>1.93</v>
+      </c>
+      <c r="M49">
+        <v>1.49</v>
+      </c>
+      <c r="N49">
+        <v>2.6</v>
+      </c>
+      <c r="O49">
+        <v>2.62</v>
+      </c>
+      <c r="P49">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="D50">
         <v>2024</v>
       </c>
       <c r="E50">
-        <v>5.92</v>
+        <v>-8.18</v>
       </c>
       <c r="F50">
-        <v>7.23</v>
+        <v>-1.68</v>
       </c>
       <c r="G50">
-        <v>-3.77</v>
+        <v>-7.81</v>
       </c>
       <c r="H50">
-        <v>8.68</v>
+        <v>2.56</v>
       </c>
       <c r="I50">
-        <v>-2.65</v>
+        <v>-7.99</v>
       </c>
       <c r="J50">
-        <v>-11.03</v>
+        <v>-12.89</v>
       </c>
       <c r="K50">
-        <v>-9.7899999999999991</v>
+        <v>-11.65</v>
       </c>
       <c r="L50">
-        <v>-5.31</v>
+        <v>-8.2200000000000006</v>
       </c>
       <c r="M50">
-        <v>-4.5</v>
+        <v>-7.09</v>
       </c>
       <c r="N50">
-        <v>-3.04</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="O50">
-        <v>-8.1</v>
+        <v>12.84</v>
       </c>
       <c r="P50">
-        <v>-5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+        <v>17.07</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="D51">
         <v>2025</v>
       </c>
       <c r="E51">
-        <v>-8</v>
+        <v>8.59</v>
       </c>
       <c r="F51">
-        <v>-7.24</v>
+        <v>10.83</v>
       </c>
       <c r="G51">
-        <v>-0.14000000000000001</v>
+        <v>16.02</v>
       </c>
       <c r="H51">
-        <v>-4.91</v>
+        <v>9.69</v>
       </c>
       <c r="I51">
-        <v>0.13</v>
+        <v>12.17</v>
       </c>
       <c r="J51">
-        <v>3.01</v>
+        <v>20.97</v>
       </c>
       <c r="K51">
-        <v>0.95</v>
-      </c>
-      <c r="L51">
-        <v>1.93</v>
+        <v>27.27</v>
       </c>
       <c r="M51">
-        <v>1.49</v>
+        <v>19.38</v>
       </c>
       <c r="N51">
-        <v>2.6</v>
+        <v>17.48</v>
       </c>
       <c r="O51">
-        <v>2.62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+        <v>7.3</v>
+      </c>
+      <c r="P51">
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="D52">
         <v>2024</v>
       </c>
       <c r="E52">
-        <v>-8.18</v>
+        <v>-2.83</v>
       </c>
       <c r="F52">
-        <v>-1.68</v>
+        <v>-0.75</v>
       </c>
       <c r="G52">
-        <v>-7.81</v>
+        <v>-3.1</v>
       </c>
       <c r="H52">
-        <v>2.56</v>
+        <v>2.36</v>
       </c>
       <c r="I52">
-        <v>-7.99</v>
+        <v>1.99</v>
       </c>
       <c r="J52">
-        <v>-12.89</v>
+        <v>-6.92</v>
       </c>
       <c r="K52">
-        <v>-11.65</v>
+        <v>-1.06</v>
       </c>
       <c r="L52">
-        <v>-8.2200000000000006</v>
-      </c>
-      <c r="M52">
-        <v>-7.09</v>
+        <v>1.59</v>
       </c>
       <c r="N52">
-        <v>4.6100000000000003</v>
+        <v>1.38</v>
       </c>
       <c r="O52">
-        <v>12.84</v>
+        <v>1.6</v>
       </c>
       <c r="P52">
-        <v>17.07</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="D53">
         <v>2025</v>
       </c>
       <c r="E53">
-        <v>8.59</v>
+        <v>5.74</v>
       </c>
       <c r="F53">
-        <v>10.83</v>
+        <v>1.78</v>
       </c>
       <c r="G53">
-        <v>16.02</v>
+        <v>5.56</v>
       </c>
       <c r="H53">
-        <v>9.69</v>
+        <v>5.39</v>
       </c>
       <c r="I53">
-        <v>12.17</v>
+        <v>0.47</v>
       </c>
       <c r="J53">
-        <v>20.97</v>
+        <v>4.75</v>
       </c>
       <c r="K53">
-        <v>27.27</v>
-      </c>
-      <c r="M53">
-        <v>19.38</v>
+        <v>12.59</v>
+      </c>
+      <c r="L53">
+        <v>1.93</v>
       </c>
       <c r="N53">
-        <v>17.48</v>
+        <v>2.14</v>
       </c>
       <c r="O53">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54">
-        <v>2024</v>
-      </c>
-      <c r="E54">
-        <v>-2.83</v>
-      </c>
-      <c r="F54">
-        <v>-0.75</v>
-      </c>
-      <c r="G54">
-        <v>-3.1</v>
-      </c>
-      <c r="H54">
-        <v>2.36</v>
-      </c>
-      <c r="I54">
+        <v>0.27</v>
+      </c>
+      <c r="P53">
         <v>1.99</v>
-      </c>
-      <c r="J54">
-        <v>-6.92</v>
-      </c>
-      <c r="K54">
-        <v>-1.06</v>
-      </c>
-      <c r="L54">
-        <v>1.59</v>
-      </c>
-      <c r="N54">
-        <v>1.38</v>
-      </c>
-      <c r="O54">
-        <v>1.6</v>
-      </c>
-      <c r="P54">
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55">
-        <v>2025</v>
-      </c>
-      <c r="E55">
-        <v>5.74</v>
-      </c>
-      <c r="F55">
-        <v>1.78</v>
-      </c>
-      <c r="G55">
-        <v>5.56</v>
-      </c>
-      <c r="H55">
-        <v>5.39</v>
-      </c>
-      <c r="I55">
-        <v>0.47</v>
-      </c>
-      <c r="J55">
-        <v>4.75</v>
-      </c>
-      <c r="K55">
-        <v>12.59</v>
-      </c>
-      <c r="L55">
-        <v>1.93</v>
-      </c>
-      <c r="N55">
-        <v>2.14</v>
-      </c>
-      <c r="O55">
-        <v>0.27</v>
       </c>
     </row>
   </sheetData>
@@ -5063,13 +5096,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>162</v>
       </c>
@@ -5113,7 +5146,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -5157,7 +5190,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -5165,19 +5198,19 @@
         <v>2025</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E3">
-        <v>1.0195000000000001</v>
+        <v>1.0207999999999999</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3">
-        <v>0.91198202920342375</v>
+        <v>0.89644907764604609</v>
       </c>
       <c r="H3" t="s">
         <v>175</v>
@@ -5189,16 +5222,60 @@
         <v>177</v>
       </c>
       <c r="K3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L3" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3">
+        <v>0.3</v>
+      </c>
+      <c r="N3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4">
+        <v>2025</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>-0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.9993631999999999</v>
+      </c>
+      <c r="F4">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>1.321361087941616</v>
+      </c>
+      <c r="H4" t="s">
         <v>180</v>
       </c>
-      <c r="M3">
-        <v>0.2</v>
-      </c>
-      <c r="N3">
-        <v>3.8</v>
+      <c r="I4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L4" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4">
+        <v>-2.7</v>
+      </c>
+      <c r="N4">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -5212,9 +5289,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>162</v>
       </c>
@@ -5258,7 +5335,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -5266,19 +5343,19 @@
         <v>2024</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>-2.2999999999999998</v>
+        <v>-2.1</v>
       </c>
       <c r="E2">
-        <v>0.97709999999999997</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="F2">
         <v>26</v>
       </c>
       <c r="G2">
-        <v>1.001137788558742</v>
+        <v>0.96764651594296858</v>
       </c>
       <c r="H2" t="s">
         <v>175</v>
@@ -5290,19 +5367,19 @@
         <v>177</v>
       </c>
       <c r="K2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M2">
-        <v>-4.3</v>
+        <v>-4</v>
       </c>
       <c r="N2">
-        <v>-0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -5310,19 +5387,19 @@
         <v>2025</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E3">
-        <v>1.0195000000000001</v>
+        <v>1.0207999999999999</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3">
-        <v>0.91198202920342375</v>
+        <v>0.89644907764604609</v>
       </c>
       <c r="H3" t="s">
         <v>175</v>
@@ -5334,19 +5411,19 @@
         <v>177</v>
       </c>
       <c r="K3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="N3">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -5354,40 +5431,40 @@
         <v>2025</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>-0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="E4">
-        <v>0.99615345</v>
+        <v>0.9993631999999999</v>
       </c>
       <c r="F4">
         <v>26</v>
       </c>
       <c r="G4">
-        <v>1.35494839432035</v>
+        <v>1.321361087941616</v>
       </c>
       <c r="H4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" t="s">
         <v>181</v>
-      </c>
-      <c r="I4" t="s">
-        <v>182</v>
       </c>
       <c r="J4" t="s">
         <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M4">
-        <v>-3.1</v>
+        <v>-2.7</v>
       </c>
       <c r="N4">
-        <v>2.2999999999999998</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -5397,16 +5474,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="20.7265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>165</v>
       </c>
@@ -5417,13 +5494,13 @@
         <v>166</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>173</v>
@@ -5432,22 +5509,22 @@
         <v>174</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.97690990001742462</v>
       </c>
@@ -5473,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J2" s="2">
         <v>45627</v>
@@ -5485,10 +5562,10 @@
         <v>2024</v>
       </c>
       <c r="M2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.97727067764172348</v>
       </c>
@@ -5514,7 +5591,7 @@
         <v>0.1</v>
       </c>
       <c r="I3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J3" s="2">
         <v>45658</v>
@@ -5526,10 +5603,10 @@
         <v>2025</v>
       </c>
       <c r="M3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.97420736895427706</v>
       </c>
@@ -5555,7 +5632,7 @@
         <v>-0.1</v>
       </c>
       <c r="I4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J4" s="2">
         <v>45689</v>
@@ -5567,10 +5644,10 @@
         <v>2025</v>
       </c>
       <c r="M4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.97585404487617367</v>
       </c>
@@ -5596,7 +5673,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J5" s="2">
         <v>45717</v>
@@ -5608,10 +5685,10 @@
         <v>2025</v>
       </c>
       <c r="M5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.97411214263331747</v>
       </c>
@@ -5637,7 +5714,7 @@
         <v>-0.2</v>
       </c>
       <c r="I6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J6" s="2">
         <v>45748</v>
@@ -5649,10 +5726,10 @@
         <v>2025</v>
       </c>
       <c r="M6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.97584822450743247</v>
       </c>
@@ -5678,7 +5755,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J7" s="2">
         <v>45778</v>
@@ -5690,10 +5767,10 @@
         <v>2025</v>
       </c>
       <c r="M7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.98326688446718169</v>
       </c>
@@ -5719,7 +5796,7 @@
         <v>0.8</v>
       </c>
       <c r="I8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J8" s="2">
         <v>45809</v>
@@ -5731,10 +5808,10 @@
         <v>2025</v>
       </c>
       <c r="M8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.99300094751402368</v>
       </c>
@@ -5760,7 +5837,7 @@
         <v>2.1</v>
       </c>
       <c r="I9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J9" s="2">
         <v>45839</v>
@@ -5772,10 +5849,10 @@
         <v>2025</v>
       </c>
       <c r="M9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.99354952738487901</v>
       </c>
@@ -5801,7 +5878,7 @@
         <v>2.1</v>
       </c>
       <c r="I10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J10" s="2">
         <v>45870</v>
@@ -5813,10 +5890,10 @@
         <v>2025</v>
       </c>
       <c r="M10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.99915322495263881</v>
       </c>
@@ -5842,7 +5919,7 @@
         <v>2.7</v>
       </c>
       <c r="I11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J11" s="2">
         <v>45901</v>
@@ -5854,10 +5931,10 @@
         <v>2025</v>
       </c>
       <c r="M11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.0014027511218691</v>
       </c>
@@ -5883,7 +5960,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J12" s="2">
         <v>45931</v>
@@ -5895,10 +5972,10 @@
         <v>2025</v>
       </c>
       <c r="M12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.004100693421716</v>
       </c>
@@ -5924,7 +6001,7 @@
         <v>3.3</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J13" s="2">
         <v>45962</v>
@@ -5936,7 +6013,89 @@
         <v>2025</v>
       </c>
       <c r="M13" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.006574391191835</v>
+      </c>
+      <c r="B14">
+        <v>0.6574391191834561</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>16.1890479828708</v>
+      </c>
+      <c r="E14">
+        <v>5.5867564845595759</v>
+      </c>
+      <c r="F14">
+        <v>1.3885102389669679</v>
+      </c>
+      <c r="G14">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H14">
+        <v>3.6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>202</v>
+      </c>
+      <c r="J14" s="2">
+        <v>45992</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>2025</v>
+      </c>
+      <c r="M14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.98673003268731097</v>
+      </c>
+      <c r="B15">
+        <v>-1.3269967312689031</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>12.53309682820035</v>
+      </c>
+      <c r="E15">
+        <v>4.2405725209462908</v>
+      </c>
+      <c r="F15">
+        <v>1.1978303072094849</v>
+      </c>
+      <c r="G15">
+        <v>-3.9</v>
+      </c>
+      <c r="H15">
+        <v>1.2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>203</v>
+      </c>
+      <c r="J15" s="2">
+        <v>45992</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>2025</v>
+      </c>
+      <c r="M15" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>